<commit_message>
working progress on circuit and layout. using MOSFETs for ignition circuit
</commit_message>
<xml_diff>
--- a/BOM parts list.xlsx
+++ b/BOM parts list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\jalouke\Launch_Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66FF85D-41CC-4872-BDE3-B807B359F90B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24317DC2-01F0-4F64-9986-D548D419A072}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10020" xr2:uid="{271B49B4-5EB4-4576-B69B-FC9B597F330F}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -42,40 +39,154 @@
     <t>Key Switch</t>
   </si>
   <si>
-    <t>KO103C701</t>
-  </si>
-  <si>
-    <t>Manufacturer P/N</t>
-  </si>
-  <si>
-    <t>E-Switch</t>
-  </si>
-  <si>
     <t>Vendor P/N</t>
   </si>
   <si>
     <t>Vendor</t>
   </si>
   <si>
-    <t>EG2623-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/e-switch/KO103C701/EG2623-ND/502087</t>
-  </si>
-  <si>
-    <t>4 circuit barrier strip</t>
-  </si>
-  <si>
-    <t>Molex, LLC</t>
-  </si>
-  <si>
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>WM5751-ND</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/product-detail/en/molex-llc/0387216704/WM5751-ND/362468</t>
+    <t>https://www.digikey.com/product-detail/en/nkk-switches/CKM12BFW01-001/360-3204-ND/761205</t>
+  </si>
+  <si>
+    <t>360-3204-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/molex-llc/0387217303/WM24401-ND/4478315</t>
+  </si>
+  <si>
+    <t>WM24401-ND</t>
+  </si>
+  <si>
+    <t>3 circuit barrier strip</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Shielded-Stranded-Conductor-Security-Burglar/dp/B077MLGLDY/ref=sr_1_5?s=electronics&amp;ie=UTF8&amp;qid=1546191887&amp;sr=1-5&amp;keywords=2%2Bconductor%2Bshielded%2Bcable&amp;th=1</t>
+  </si>
+  <si>
+    <t>500ft 22/2 sheilded cable</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/lumex-opto-components-inc/SSI-LXH600ID-150/67-1188-ND/145088</t>
+  </si>
+  <si>
+    <t>67-1188-ND</t>
+  </si>
+  <si>
+    <t>Panel Mount LED</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/nkk-switches/KB25RKW01-5C-JC/360-2005-ND/1007062</t>
+  </si>
+  <si>
+    <t>360-2005-ND</t>
+  </si>
+  <si>
+    <t>Pushbutton switch</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/nkk-switches/AT4024/360-1006-ND/379093</t>
+  </si>
+  <si>
+    <t>360-1006-ND</t>
+  </si>
+  <si>
+    <t>switch cover</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/c-k/A12405RNZG/CKN11082-ND/3751956</t>
+  </si>
+  <si>
+    <t>rotary switch</t>
+  </si>
+  <si>
+    <t>CKN11082-ND</t>
+  </si>
+  <si>
+    <t>rotary knob</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9998</t>
+  </si>
+  <si>
+    <t>sparkfun</t>
+  </si>
+  <si>
+    <t>COM-09998</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/11138</t>
+  </si>
+  <si>
+    <t>Rocker Switch</t>
+  </si>
+  <si>
+    <t>COM-11138</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/recom-power/R-78E3.3-0.5/945-1661-5-ND/3593412</t>
+  </si>
+  <si>
+    <t>945-1661-5-ND</t>
+  </si>
+  <si>
+    <t>DC-DC Converter</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/536</t>
+  </si>
+  <si>
+    <t>COM-00536</t>
+  </si>
+  <si>
+    <t>16MHz Crystal</t>
+  </si>
+  <si>
+    <t>P-ch Mosfet</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/on-semiconductor/FQP8P10/FQP8P10FS-ND/1053762</t>
+  </si>
+  <si>
+    <t>FQP8P10FS-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/microchip-technology/2N7000-G/2N7000-G-ND/4902350</t>
+  </si>
+  <si>
+    <t>2N7000-G-ND</t>
+  </si>
+  <si>
+    <t>N-ch Mosfet</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/panasonic-electronic-components/ECE-A1EKS100/P975-ND/160555</t>
+  </si>
+  <si>
+    <t>P975-ND</t>
+  </si>
+  <si>
+    <t>10uF cap</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/comchip-technology/1N4007-G/641-1312-1-ND/1979677</t>
+  </si>
+  <si>
+    <t>641-1312-1-ND</t>
+  </si>
+  <si>
+    <t>1N4007-G Diode</t>
   </si>
 </sst>
 </file>
@@ -83,15 +194,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF777777"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,10 +237,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,88 +559,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3044430A-1187-44BB-B3A8-3907AF7139C0}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.36328125" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
+      <c r="B1" t="s">
+        <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.86</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>28.95</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>10.8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8.19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="E10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2">
-        <v>5.71</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2">
-        <v>387216704</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>3.19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
+      <c r="E13" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>